<commit_message>
leetcode solved insert remove getrandom in O(1)
</commit_message>
<xml_diff>
--- a/LeetCode/Random.xlsx
+++ b/LeetCode/Random.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Coding\Programming Language\DSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Competetive_Programming\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E7083F-621F-48A3-8093-47E4944FD8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A33B4F7-C8E5-4DAB-9A2D-48E20BAC1410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="1447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="1448">
   <si>
     <t>https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/middle-of-a-linked-list/ojquestion</t>
   </si>
@@ -4372,6 +4372,9 @@
   </si>
   <si>
     <t>Imp</t>
+  </si>
+  <si>
+    <t>solve later alos</t>
   </si>
 </sst>
 </file>
@@ -4829,7 +4832,7 @@
   <dimension ref="A1:N731"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5251,9 +5254,11 @@
         <v>Insert delete GetRand O(1)</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>1422</v>
-      </c>
-      <c r="E24" s="3"/>
+        <v>1423</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>1447</v>
+      </c>
       <c r="M24" t="s">
         <v>845</v>
       </c>

</xml_diff>